<commit_message>
Additional changes required for the EMEP UNFCCC, and China (MEIC) emission inventory updates. Including changes to the emission factor pathway files for NOx, NMVOC, and CO.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR14_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_NFR14_scaling_mapping.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B386F668-0D2D-464E-9A6C-FE0D9EEAFDC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EABC500-7A0A-9E44-949B-1AEFAC142BAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="4040" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="7400" windowWidth="25600" windowHeight="13940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="102">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -323,10 +329,16 @@
     <t>Avoid imlied Nox EF dip 1986-1989</t>
   </si>
   <si>
-    <t>Problematic to lump this with stationary sectors, and probably something other than rail here, so try leaving out</t>
-  </si>
-  <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Problematic to lump this with stationary sectors, and probably something other than rail here, so try leaving out. Also includes some 1A4c</t>
+  </si>
+  <si>
+    <t>not included in official definition</t>
+  </si>
+  <si>
+    <t>This sector is large for some countries, but seems to be inconsistantly reported by country</t>
   </si>
 </sst>
 </file>
@@ -1126,16 +1138,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="5" max="6" width="41" bestFit="1" customWidth="1"/>
   </cols>
@@ -1476,99 +1488,100 @@
         <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>75</v>
+      <c r="A36" t="s">
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>98</v>
+      </c>
+      <c r="E36" t="s">
+        <v>101</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="2" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
       <c r="B43" t="s">
         <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D43" s="2"/>
     </row>
@@ -1577,7 +1590,7 @@
         <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -1586,85 +1599,100 @@
         <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
       <c r="B47" t="s">
         <v>82</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>82</v>
+      </c>
       <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C50" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="2"/>
-      <c r="C51" t="s">
-        <v>46</v>
-      </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="2"/>
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>84</v>
+        <v>59</v>
+      </c>
+      <c r="B53" t="s">
+        <v>85</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>59</v>
-      </c>
+      <c r="A54" s="4"/>
       <c r="B54" t="s">
         <v>85</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1673,29 +1701,27 @@
         <v>85</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
-      <c r="B56" t="s">
-        <v>85</v>
-      </c>
       <c r="C56" t="s">
-        <v>79</v>
-      </c>
-      <c r="E56" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
       <c r="B57" t="s">
         <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -1705,46 +1731,41 @@
         <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>85</v>
-      </c>
-      <c r="C59" t="s">
-        <v>78</v>
+      <c r="A59" t="s">
+        <v>60</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>60</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="2"/>
+      <c r="C62" s="4"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C63" s="4"/>
+      <c r="C63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
@@ -1754,11 +1775,11 @@
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
@@ -1789,6 +1810,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
+      <c r="C72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
@@ -1811,13 +1833,14 @@
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
+      <c r="A76" s="2"/>
       <c r="C76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
       <c r="C77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -1853,7 +1876,7 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
-      <c r="C82" s="2"/>
+      <c r="C82" s="1"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
@@ -1874,7 +1897,6 @@
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
-      <c r="C85" s="1"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
@@ -1886,7 +1908,6 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
-      <c r="B87" s="3"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
@@ -1896,7 +1917,6 @@
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
@@ -1905,7 +1925,7 @@
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E91" s="2"/>
+      <c r="E91" s="1"/>
       <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -1917,11 +1937,10 @@
       <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E94" s="1"/>
+      <c r="C94" s="1"/>
       <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C95" s="1"/>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -1931,10 +1950,10 @@
       <c r="F97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="2"/>
       <c r="F98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="2"/>
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -1947,10 +1966,10 @@
       <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E103" s="1"/>
       <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E104" s="1"/>
       <c r="F104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -1978,7 +1997,7 @@
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F113" s="2"/>
+      <c r="F113" s="1"/>
     </row>
     <row r="114" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F114" s="1"/>
@@ -1986,11 +2005,8 @@
     <row r="115" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F116" s="1"/>
-    </row>
-    <row r="126" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F126" s="1"/>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F125" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2065,7 +2081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>